<commit_message>
Finish Base Class Market
</commit_message>
<xml_diff>
--- a/excels/heroController.xlsx
+++ b/excels/heroController.xlsx
@@ -77,19 +77,13 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color rgb="FFCE9178"/>
-      <name val="Consolas"/>
-      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -556,142 +550,139 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1007,7 +998,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -1044,7 +1035,7 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3">
@@ -1058,7 +1049,7 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4">
@@ -1072,7 +1063,7 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5">
@@ -1086,7 +1077,7 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6">
@@ -1100,7 +1091,7 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7">
@@ -1114,7 +1105,7 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8">

</xml_diff>